<commit_message>
Feat(Maquette) : Ajout de 2 maquettes
[100] [Done]
</commit_message>
<xml_diff>
--- a/doc/m-planification-jnltrav.xlsx
+++ b/doc/m-planification-jnltrav.xlsx
@@ -5,10 +5,10 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pb17shq\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Poo\P_oo-Shoot-me-up\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCE9471-B934-4D85-B98F-70E138676BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D148DC12-2DDD-4072-9F5B-0DADDE049527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$66</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$68</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -121,16 +121,58 @@
     <t>Analyse</t>
   </si>
   <si>
-    <t>Explication du projet / Done</t>
-  </si>
-  <si>
     <t xml:space="preserve">Conseption </t>
   </si>
   <si>
-    <t>Creation des maquette / WIP</t>
-  </si>
-  <si>
-    <t>Theme fonctionalités /Done</t>
+    <t>Explication user story</t>
+  </si>
+  <si>
+    <t>Structure de projet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User story </t>
+  </si>
+  <si>
+    <t>Maquette / schema</t>
+  </si>
+  <si>
+    <t>Schema de Zone, Schema de contournement | Done</t>
+  </si>
+  <si>
+    <t>Creation des maquette | WIP</t>
+  </si>
+  <si>
+    <t>Theme fonctionalités | Done</t>
+  </si>
+  <si>
+    <t>Explication du projet | Done</t>
+  </si>
+  <si>
+    <t>Convention de commit</t>
+  </si>
+  <si>
+    <t>Ecriture des users story | Done</t>
+  </si>
+  <si>
+    <t>Demander à João (3éme) comment nomer mes commit |Done</t>
+  </si>
+  <si>
+    <t>Backlog · kanban</t>
+  </si>
+  <si>
+    <t>figma</t>
+  </si>
+  <si>
+    <t>Restructuration des dossier | Done</t>
+  </si>
+  <si>
+    <t>Exemple au tableau de commant faire | Done</t>
+  </si>
+  <si>
+    <t>Explication deplacement</t>
+  </si>
+  <si>
+    <t>explication des evitement d'obstacle| Done</t>
   </si>
 </sst>
 </file>
@@ -355,7 +397,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -434,6 +476,18 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -464,17 +518,16 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -791,21 +844,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="80.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="50.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="138.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="36" style="1" customWidth="1"/>
     <col min="8" max="16384" width="11.42578125" style="1"/>
@@ -815,10 +869,10 @@
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="31"/>
+      <c r="C1" s="23"/>
       <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
@@ -830,10 +884,10 @@
       <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="31"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="22" t="s">
         <v>4</v>
       </c>
@@ -845,10 +899,10 @@
       <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="31"/>
+      <c r="C3" s="23"/>
       <c r="D3" s="22" t="s">
         <v>7</v>
       </c>
@@ -860,12 +914,12 @@
       <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="34"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
     </row>
     <row r="5" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -888,14 +942,14 @@
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="27">
         <v>45896</v>
       </c>
       <c r="C6" s="5">
         <v>90</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E6" s="5"/>
     </row>
@@ -903,38 +957,40 @@
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="24"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="8">
         <v>45</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="24"/>
+        <v>23</v>
+      </c>
+      <c r="B8" s="28"/>
       <c r="C8" s="8">
         <v>45</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="24"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="25"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="10"/>
@@ -943,511 +999,564 @@
       <c r="A11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="26"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="28"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="32"/>
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="23">
+      <c r="A12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="27">
         <f>B6+7</f>
         <v>45903</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
+      <c r="C12" s="5">
+        <v>25</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>38</v>
+      </c>
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
+      <c r="A13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="8">
+        <v>5</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="8"/>
+    <row r="14" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="28"/>
+      <c r="C14" s="8">
+        <v>100</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
+      <c r="A15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="28"/>
+      <c r="C15" s="8">
+        <v>40</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="10">
+        <v>5</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="E16" s="10"/>
     </row>
-    <row r="17" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="28"/>
+      <c r="C17" s="10">
+        <v>5</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="10"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="28"/>
-    </row>
-    <row r="18" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="23">
+      <c r="B19" s="30"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="32"/>
+    </row>
+    <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="27">
         <f>B12+7</f>
         <v>45910</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="8"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="24"/>
+      <c r="B21" s="28"/>
       <c r="C21" s="8"/>
       <c r="D21" s="9"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
+    <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="10"/>
+    </row>
+    <row r="25" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="28"/>
-    </row>
-    <row r="24" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="23">
-        <f>B18+7</f>
+      <c r="B25" s="30"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="32"/>
+    </row>
+    <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="27">
+        <f>B20+7</f>
         <v>45917</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="8"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="24"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="8"/>
       <c r="D27" s="9"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="10"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="10"/>
-    </row>
-    <row r="29" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="12" t="s">
+    <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="10"/>
+    </row>
+    <row r="31" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="28"/>
-    </row>
-    <row r="30" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="23">
-        <f>B24+7</f>
+      <c r="B31" s="30"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="32"/>
+    </row>
+    <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="27">
+        <f>B26+7</f>
         <v>45924</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="13"/>
-    </row>
-    <row r="31" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="8"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="13"/>
     </row>
     <row r="33" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
-      <c r="B33" s="24"/>
+      <c r="B33" s="28"/>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
       <c r="E33" s="8"/>
     </row>
-    <row r="34" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
-      <c r="B34" s="25"/>
+      <c r="B34" s="28"/>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="12" t="s">
+    <row r="35" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="8"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="26"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="28"/>
-    </row>
-    <row r="36" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="23">
-        <f>B30+7</f>
+      <c r="B37" s="30"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="32"/>
+    </row>
+    <row r="38" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="27">
+        <f>B32+7</f>
         <v>45931</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="5"/>
-    </row>
-    <row r="37" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="8"/>
-    </row>
-    <row r="38" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="8"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="24"/>
+      <c r="B39" s="28"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
     </row>
-    <row r="40" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="10"/>
-    </row>
-    <row r="41" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="12" t="s">
+    <row r="40" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="8"/>
+    </row>
+    <row r="42" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="10"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="10"/>
+    </row>
+    <row r="43" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="26"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="28"/>
-    </row>
-    <row r="42" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="23">
-        <f>B36+7</f>
+      <c r="B43" s="30"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="32"/>
+    </row>
+    <row r="44" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="27">
+        <f>B38+7</f>
         <v>45938</v>
       </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="5"/>
-    </row>
-    <row r="43" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="8"/>
-    </row>
-    <row r="44" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="8"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
-      <c r="B45" s="24"/>
+      <c r="B45" s="28"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="10"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="10"/>
-    </row>
-    <row r="47" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="12" t="s">
+    <row r="46" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="8"/>
+    </row>
+    <row r="48" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="10"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="10"/>
+    </row>
+    <row r="49" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="26"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="28"/>
-    </row>
-    <row r="48" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="23">
-        <f>B42+7</f>
+      <c r="B49" s="30"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="32"/>
+    </row>
+    <row r="50" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="27">
+        <f>B44+7</f>
         <v>45945</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="8"/>
-    </row>
-    <row r="50" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="8"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="5"/>
     </row>
     <row r="51" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
-      <c r="B51" s="24"/>
+      <c r="B51" s="28"/>
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
       <c r="E51" s="8"/>
     </row>
-    <row r="52" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="10"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="10"/>
-    </row>
-    <row r="53" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="12" t="s">
+    <row r="52" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="8"/>
+    </row>
+    <row r="53" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="7"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="8"/>
+    </row>
+    <row r="54" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="10"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="10"/>
+    </row>
+    <row r="55" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="26"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="28"/>
-    </row>
-    <row r="54" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="23">
-        <f>B48+7</f>
+      <c r="B55" s="30"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="32"/>
+    </row>
+    <row r="56" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="27">
+        <f>B50+7</f>
         <v>45952</v>
       </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="5"/>
-    </row>
-    <row r="55" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="24"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="8"/>
-    </row>
-    <row r="56" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="24"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="8"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="5"/>
     </row>
     <row r="57" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
-      <c r="B57" s="24"/>
+      <c r="B57" s="28"/>
       <c r="C57" s="8"/>
       <c r="D57" s="9"/>
       <c r="E57" s="8"/>
     </row>
-    <row r="58" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="10"/>
-      <c r="B58" s="25"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="10"/>
-    </row>
-    <row r="59" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="12" t="s">
+    <row r="58" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+      <c r="B58" s="28"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="8"/>
+    </row>
+    <row r="59" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="8"/>
+    </row>
+    <row r="60" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="10"/>
+      <c r="B60" s="29"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="10"/>
+    </row>
+    <row r="61" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="26"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="27"/>
-      <c r="E59" s="28"/>
-    </row>
-    <row r="60" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
-      <c r="B60" s="23">
-        <f>B54+7</f>
+      <c r="B61" s="30"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="32"/>
+    </row>
+    <row r="62" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="13"/>
+      <c r="B62" s="27">
+        <f>B56+7</f>
         <v>45959</v>
       </c>
-      <c r="C60" s="13"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="13"/>
-    </row>
-    <row r="61" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="8"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="8"/>
-    </row>
-    <row r="62" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="8"/>
-      <c r="B62" s="24"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="8"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="13"/>
     </row>
     <row r="63" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
-      <c r="B63" s="24"/>
+      <c r="B63" s="28"/>
       <c r="C63" s="8"/>
       <c r="D63" s="9"/>
       <c r="E63" s="8"/>
     </row>
-    <row r="64" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
-      <c r="B64" s="25"/>
+      <c r="B64" s="28"/>
       <c r="C64" s="8"/>
       <c r="D64" s="9"/>
       <c r="E64" s="8"/>
     </row>
-    <row r="65" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="12" t="s">
+    <row r="65" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="8"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="8"/>
+    </row>
+    <row r="66" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="8"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="8"/>
+    </row>
+    <row r="67" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B65" s="26"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="27"/>
-      <c r="E65" s="28"/>
-    </row>
-    <row r="66" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="29" t="s">
+      <c r="B67" s="30"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="32"/>
+    </row>
+    <row r="68" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B66" s="30"/>
-      <c r="C66" s="15">
-        <f>MROUND(SUM(C6:C65) /60,0.2)</f>
-        <v>3</v>
-      </c>
-      <c r="D66" s="16"/>
-      <c r="E66" s="17"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="18" t="s">
+      <c r="B68" s="34"/>
+      <c r="C68" s="15">
+        <f>MROUND(SUM(C6:C67) /60,0.2)</f>
+        <v>6</v>
+      </c>
+      <c r="D68" s="16"/>
+      <c r="E68" s="17"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="18"/>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B50:B54"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B61:E61"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B60:B64"/>
-    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B62:B66"/>
+    <mergeCell ref="B43:E43"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="B42:B46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B48:B52"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B54:B58"/>
-    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="B37:E37"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C54:C58 C48:C52 C36:C40 C42:C46 C18:C22 B6 C12:C16 C24:C28 C30:C34 C60:C64 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C56:C60 C50:C54 C38:C42 C44:C48 C20:C24 B6 C12:C18 C26:C30 C32:C36 C62:C66 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B12:B16 B54:B58 B18:B22 B24:B28 B30:B34 B36:B40 B42:B46 B48:B52 B60:B64" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B12:B18 B56:B60 B20:B24 B26:B30 B32:B36 B38:B42 B44:B48 B50:B54 B62:B66" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
       <formula1>45261</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E14" r:id="rId1" display="https://github.com/users/djdams1/projects/2/views/1" xr:uid="{9B5D630F-F3CA-4BE9-BE1C-70C324722A61}"/>
+    <hyperlink ref="E15" r:id="rId2" xr:uid="{B9AB9621-1570-41D7-A2C6-6FF27F13DC4B}"/>
+    <hyperlink ref="E8" r:id="rId3" xr:uid="{8FEF73A3-AAC4-4357-865C-F89C66FF328B}"/>
+  </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="50" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="37" orientation="portrait" r:id="rId4"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Etml_font,Normal"&amp;22ETML&amp;R&amp;G</oddHeader>
     <oddFooter>&amp;L&amp;14&amp;D&amp;R&amp;14Journal</oddFooter>
   </headerFooter>
-  <legacyDrawingHF r:id="rId2"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="17" max="16383" man="1"/>
+  </rowBreaks>
+  <legacyDrawingHF r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -1690,6 +1799,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1702,14 +1820,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1728,6 +1838,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
chose(gitjournal) : ajoute gitjournal au projet
</commit_message>
<xml_diff>
--- a/doc/m-planification-jnltrav.xlsx
+++ b/doc/m-planification-jnltrav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Poo\P_oo-Shoot-me-up\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D148DC12-2DDD-4072-9F5B-0DADDE049527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118AAE72-38B7-4D49-A392-5B02C1F3BE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -157,9 +157,6 @@
     <t>Demander à João (3éme) comment nomer mes commit |Done</t>
   </si>
   <si>
-    <t>Backlog · kanban</t>
-  </si>
-  <si>
     <t>figma</t>
   </si>
   <si>
@@ -173,6 +170,15 @@
   </si>
   <si>
     <t>explication des evitement d'obstacle| Done</t>
+  </si>
+  <si>
+    <t>feedback, release, tests d'acceptance, journal, auto-éval</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>score, colision, obstacles, tire des ennemis, tire des joueur, ennemis, joueur | Backlog · kanban</t>
   </si>
 </sst>
 </file>
@@ -236,7 +242,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -389,6 +395,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -397,7 +412,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -476,6 +491,47 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -488,46 +544,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -844,13 +862,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -865,14 +883,14 @@
     <col min="8" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="23"/>
+      <c r="C1" s="34"/>
       <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
@@ -880,14 +898,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="23"/>
+      <c r="C2" s="34"/>
       <c r="D2" s="22" t="s">
         <v>4</v>
       </c>
@@ -895,14 +913,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="23"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="22" t="s">
         <v>7</v>
       </c>
@@ -910,18 +928,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="26"/>
-    </row>
-    <row r="5" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="37"/>
+    </row>
+    <row r="5" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -938,11 +956,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="26">
         <v>45896</v>
       </c>
       <c r="C6" s="5">
@@ -953,11 +971,11 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="28"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="8">
         <v>45</v>
       </c>
@@ -966,49 +984,49 @@
       </c>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="28"/>
+      <c r="B8" s="27"/>
       <c r="C8" s="8">
         <v>45</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="28"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="29"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="10"/>
     </row>
-    <row r="11" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32"/>
-    </row>
-    <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="31"/>
+    </row>
+    <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="27">
+      <c r="B12" s="26">
         <f>B6+7</f>
         <v>45903</v>
       </c>
@@ -1016,58 +1034,59 @@
         <v>25</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="28"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="8">
         <v>5</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="28"/>
+      <c r="B14" s="27"/>
       <c r="C14" s="8">
         <v>100</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="38"/>
+    </row>
+    <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="28"/>
+      <c r="B15" s="27"/>
       <c r="C15" s="8">
         <v>40</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
+      <c r="E15" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="28"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="10">
         <v>5</v>
       </c>
@@ -1077,21 +1096,21 @@
       <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="28"/>
+      <c r="A17" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="27"/>
       <c r="C17" s="10">
         <v>5</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17" s="10"/>
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
-      <c r="B18" s="29"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
       <c r="E18" s="10"/>
@@ -1100,45 +1119,51 @@
       <c r="A19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="32"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="31"/>
     </row>
     <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="27">
+      <c r="A20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="26">
         <f>B12+7</f>
         <v>45910</v>
       </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="5">
+        <v>40</v>
+      </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="5"/>
+      <c r="E20" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
-      <c r="B21" s="28"/>
+      <c r="B21" s="27"/>
       <c r="C21" s="8"/>
       <c r="D21" s="9"/>
       <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
-      <c r="B22" s="28"/>
+      <c r="B22" s="27"/>
       <c r="C22" s="8"/>
       <c r="D22" s="9"/>
       <c r="E22" s="8"/>
     </row>
     <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
-      <c r="B23" s="28"/>
+      <c r="B23" s="27"/>
       <c r="C23" s="8"/>
       <c r="D23" s="9"/>
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
-      <c r="B24" s="29"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
       <c r="E24" s="10"/>
@@ -1147,14 +1172,14 @@
       <c r="A25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="32"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="31"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="27">
+      <c r="B26" s="26">
         <f>B20+7</f>
         <v>45917</v>
       </c>
@@ -1164,28 +1189,28 @@
     </row>
     <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="28"/>
+      <c r="B27" s="27"/>
       <c r="C27" s="8"/>
       <c r="D27" s="9"/>
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
-      <c r="B28" s="28"/>
+      <c r="B28" s="27"/>
       <c r="C28" s="8"/>
       <c r="D28" s="9"/>
       <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
-      <c r="B29" s="28"/>
+      <c r="B29" s="27"/>
       <c r="C29" s="8"/>
       <c r="D29" s="9"/>
       <c r="E29" s="8"/>
     </row>
     <row r="30" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
-      <c r="B30" s="29"/>
+      <c r="B30" s="28"/>
       <c r="C30" s="10"/>
       <c r="D30" s="11"/>
       <c r="E30" s="10"/>
@@ -1194,14 +1219,14 @@
       <c r="A31" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="32"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="31"/>
     </row>
     <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
-      <c r="B32" s="27">
+      <c r="B32" s="26">
         <f>B26+7</f>
         <v>45924</v>
       </c>
@@ -1211,28 +1236,28 @@
     </row>
     <row r="33" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
-      <c r="B33" s="28"/>
+      <c r="B33" s="27"/>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
       <c r="E33" s="8"/>
     </row>
     <row r="34" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
-      <c r="B34" s="28"/>
+      <c r="B34" s="27"/>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
       <c r="E34" s="8"/>
     </row>
     <row r="35" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
-      <c r="B35" s="28"/>
+      <c r="B35" s="27"/>
       <c r="C35" s="8"/>
       <c r="D35" s="9"/>
       <c r="E35" s="8"/>
     </row>
     <row r="36" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
-      <c r="B36" s="29"/>
+      <c r="B36" s="28"/>
       <c r="C36" s="8"/>
       <c r="D36" s="9"/>
       <c r="E36" s="8"/>
@@ -1241,14 +1266,14 @@
       <c r="A37" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="32"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="31"/>
     </row>
     <row r="38" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="27">
+      <c r="B38" s="26">
         <f>B32+7</f>
         <v>45931</v>
       </c>
@@ -1258,28 +1283,28 @@
     </row>
     <row r="39" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="28"/>
+      <c r="B39" s="27"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="28"/>
+      <c r="B40" s="27"/>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="28"/>
+      <c r="B41" s="27"/>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
-      <c r="B42" s="29"/>
+      <c r="B42" s="28"/>
       <c r="C42" s="10"/>
       <c r="D42" s="11"/>
       <c r="E42" s="10"/>
@@ -1288,14 +1313,14 @@
       <c r="A43" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="30"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="32"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="31"/>
     </row>
     <row r="44" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
-      <c r="B44" s="27">
+      <c r="B44" s="26">
         <f>B38+7</f>
         <v>45938</v>
       </c>
@@ -1305,28 +1330,28 @@
     </row>
     <row r="45" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
-      <c r="B45" s="28"/>
+      <c r="B45" s="27"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
       <c r="E45" s="8"/>
     </row>
     <row r="46" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
-      <c r="B46" s="28"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="8"/>
       <c r="D46" s="9"/>
       <c r="E46" s="8"/>
     </row>
     <row r="47" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
-      <c r="B47" s="28"/>
+      <c r="B47" s="27"/>
       <c r="C47" s="8"/>
       <c r="D47" s="9"/>
       <c r="E47" s="8"/>
     </row>
     <row r="48" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="10"/>
-      <c r="B48" s="29"/>
+      <c r="B48" s="28"/>
       <c r="C48" s="10"/>
       <c r="D48" s="11"/>
       <c r="E48" s="10"/>
@@ -1335,14 +1360,14 @@
       <c r="A49" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="30"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="32"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="31"/>
     </row>
     <row r="50" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
-      <c r="B50" s="27">
+      <c r="B50" s="26">
         <f>B44+7</f>
         <v>45945</v>
       </c>
@@ -1352,28 +1377,28 @@
     </row>
     <row r="51" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
-      <c r="B51" s="28"/>
+      <c r="B51" s="27"/>
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
       <c r="E51" s="8"/>
     </row>
     <row r="52" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
-      <c r="B52" s="28"/>
+      <c r="B52" s="27"/>
       <c r="C52" s="8"/>
       <c r="D52" s="9"/>
       <c r="E52" s="8"/>
     </row>
     <row r="53" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
-      <c r="B53" s="28"/>
+      <c r="B53" s="27"/>
       <c r="C53" s="8"/>
       <c r="D53" s="9"/>
       <c r="E53" s="8"/>
     </row>
     <row r="54" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="10"/>
-      <c r="B54" s="29"/>
+      <c r="B54" s="28"/>
       <c r="C54" s="10"/>
       <c r="D54" s="11"/>
       <c r="E54" s="10"/>
@@ -1382,14 +1407,14 @@
       <c r="A55" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="32"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="31"/>
     </row>
     <row r="56" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
-      <c r="B56" s="27">
+      <c r="B56" s="26">
         <f>B50+7</f>
         <v>45952</v>
       </c>
@@ -1399,28 +1424,28 @@
     </row>
     <row r="57" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
-      <c r="B57" s="28"/>
+      <c r="B57" s="27"/>
       <c r="C57" s="8"/>
       <c r="D57" s="9"/>
       <c r="E57" s="8"/>
     </row>
     <row r="58" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
-      <c r="B58" s="28"/>
+      <c r="B58" s="27"/>
       <c r="C58" s="8"/>
       <c r="D58" s="9"/>
       <c r="E58" s="8"/>
     </row>
     <row r="59" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
-      <c r="B59" s="28"/>
+      <c r="B59" s="27"/>
       <c r="C59" s="8"/>
       <c r="D59" s="9"/>
       <c r="E59" s="8"/>
     </row>
     <row r="60" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="10"/>
-      <c r="B60" s="29"/>
+      <c r="B60" s="28"/>
       <c r="C60" s="10"/>
       <c r="D60" s="11"/>
       <c r="E60" s="10"/>
@@ -1429,14 +1454,14 @@
       <c r="A61" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B61" s="30"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="32"/>
+      <c r="B61" s="29"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="31"/>
     </row>
     <row r="62" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
-      <c r="B62" s="27">
+      <c r="B62" s="26">
         <f>B56+7</f>
         <v>45959</v>
       </c>
@@ -1446,28 +1471,28 @@
     </row>
     <row r="63" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
-      <c r="B63" s="28"/>
+      <c r="B63" s="27"/>
       <c r="C63" s="8"/>
       <c r="D63" s="9"/>
       <c r="E63" s="8"/>
     </row>
     <row r="64" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
-      <c r="B64" s="28"/>
+      <c r="B64" s="27"/>
       <c r="C64" s="8"/>
       <c r="D64" s="9"/>
       <c r="E64" s="8"/>
     </row>
     <row r="65" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
-      <c r="B65" s="28"/>
+      <c r="B65" s="27"/>
       <c r="C65" s="8"/>
       <c r="D65" s="9"/>
       <c r="E65" s="8"/>
     </row>
     <row r="66" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8"/>
-      <c r="B66" s="29"/>
+      <c r="B66" s="28"/>
       <c r="C66" s="8"/>
       <c r="D66" s="9"/>
       <c r="E66" s="8"/>
@@ -1476,19 +1501,19 @@
       <c r="A67" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B67" s="30"/>
-      <c r="C67" s="31"/>
-      <c r="D67" s="31"/>
-      <c r="E67" s="32"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="30"/>
+      <c r="D67" s="30"/>
+      <c r="E67" s="31"/>
     </row>
     <row r="68" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="33" t="s">
+      <c r="A68" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B68" s="34"/>
+      <c r="B68" s="33"/>
       <c r="C68" s="15">
         <f>MROUND(SUM(C6:C67) /60,0.2)</f>
-        <v>6</v>
+        <v>6.6000000000000005</v>
       </c>
       <c r="D68" s="16"/>
       <c r="E68" s="17"/>
@@ -1503,15 +1528,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B50:B54"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B61:E61"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -1528,6 +1544,15 @@
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="B32:B36"/>
     <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B50:B54"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B61:E61"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C56:C60 C50:C54 C38:C42 C44:C48 C20:C24 B6 C12:C18 C26:C30 C32:C36 C62:C66 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
@@ -1538,7 +1563,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E14" r:id="rId1" display="https://github.com/users/djdams1/projects/2/views/1" xr:uid="{9B5D630F-F3CA-4BE9-BE1C-70C324722A61}"/>
+    <hyperlink ref="E14" r:id="rId1" display="| Backlog · kanban" xr:uid="{9B5D630F-F3CA-4BE9-BE1C-70C324722A61}"/>
     <hyperlink ref="E15" r:id="rId2" xr:uid="{B9AB9621-1570-41D7-A2C6-6FF27F13DC4B}"/>
     <hyperlink ref="E8" r:id="rId3" xr:uid="{8FEF73A3-AAC4-4357-865C-F89C66FF328B}"/>
   </hyperlinks>
@@ -1557,6 +1582,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -1799,15 +1833,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1820,6 +1845,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1838,14 +1871,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
chore(Journal de travail) : mets a jour le journal de travail
</commit_message>
<xml_diff>
--- a/doc/m-planification-jnltrav.xlsx
+++ b/doc/m-planification-jnltrav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Poo\P_oo-Shoot-me-up\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118AAE72-38B7-4D49-A392-5B02C1F3BE70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339B5419-18DC-4C15-A287-B9103762B327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>score, colision, obstacles, tire des ennemis, tire des joueur, ennemis, joueur | Backlog · kanban</t>
+  </si>
+  <si>
+    <t>Reprise des user story pour satisfaire au commantaire</t>
   </si>
 </sst>
 </file>
@@ -502,6 +505,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -531,21 +549,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -865,10 +868,10 @@
   <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -887,10 +890,10 @@
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
@@ -902,10 +905,10 @@
       <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="34"/>
+      <c r="C2" s="27"/>
       <c r="D2" s="22" t="s">
         <v>4</v>
       </c>
@@ -917,10 +920,10 @@
       <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="22" t="s">
         <v>7</v>
       </c>
@@ -932,12 +935,12 @@
       <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="37"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -960,7 +963,7 @@
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="31">
         <v>45896</v>
       </c>
       <c r="C6" s="5">
@@ -975,7 +978,7 @@
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="27"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="8">
         <v>45</v>
       </c>
@@ -988,7 +991,7 @@
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="27"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="8">
         <v>45</v>
       </c>
@@ -1001,14 +1004,14 @@
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="27"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="28"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="10"/>
@@ -1017,16 +1020,16 @@
       <c r="A11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="31"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="26">
+      <c r="B12" s="31">
         <f>B6+7</f>
         <v>45903</v>
       </c>
@@ -1042,7 +1045,7 @@
       <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="27"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="8">
         <v>5</v>
       </c>
@@ -1055,7 +1058,7 @@
       <c r="A14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="27"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="8">
         <v>100</v>
       </c>
@@ -1065,13 +1068,13 @@
       <c r="E14" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="38"/>
+      <c r="F14" s="26"/>
     </row>
     <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="27"/>
+      <c r="B15" s="32"/>
       <c r="C15" s="8">
         <v>40</v>
       </c>
@@ -1086,7 +1089,7 @@
       <c r="A16" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="27"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="10">
         <v>5</v>
       </c>
@@ -1099,7 +1102,7 @@
       <c r="A17" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="27"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="10">
         <v>5</v>
       </c>
@@ -1110,7 +1113,7 @@
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
-      <c r="B18" s="28"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
       <c r="E18" s="10"/>
@@ -1119,16 +1122,16 @@
       <c r="A19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="31"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="36"/>
     </row>
     <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="26">
+      <c r="B20" s="31">
         <f>B12+7</f>
         <v>45910</v>
       </c>
@@ -1141,29 +1144,35 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="8"/>
+      <c r="A21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="32"/>
+      <c r="C21" s="8">
+        <v>30</v>
+      </c>
       <c r="D21" s="9"/>
-      <c r="E21" s="8"/>
+      <c r="E21" s="8" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
-      <c r="B22" s="27"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="8"/>
       <c r="D22" s="9"/>
       <c r="E22" s="8"/>
     </row>
     <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
-      <c r="B23" s="27"/>
+      <c r="B23" s="32"/>
       <c r="C23" s="8"/>
       <c r="D23" s="9"/>
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
-      <c r="B24" s="28"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
       <c r="E24" s="10"/>
@@ -1172,14 +1181,14 @@
       <c r="A25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="31"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="36"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="26">
+      <c r="B26" s="31">
         <f>B20+7</f>
         <v>45917</v>
       </c>
@@ -1189,28 +1198,28 @@
     </row>
     <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="27"/>
+      <c r="B27" s="32"/>
       <c r="C27" s="8"/>
       <c r="D27" s="9"/>
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
-      <c r="B28" s="27"/>
+      <c r="B28" s="32"/>
       <c r="C28" s="8"/>
       <c r="D28" s="9"/>
       <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
-      <c r="B29" s="27"/>
+      <c r="B29" s="32"/>
       <c r="C29" s="8"/>
       <c r="D29" s="9"/>
       <c r="E29" s="8"/>
     </row>
     <row r="30" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
-      <c r="B30" s="28"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="10"/>
       <c r="D30" s="11"/>
       <c r="E30" s="10"/>
@@ -1219,14 +1228,14 @@
       <c r="A31" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="31"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="36"/>
     </row>
     <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
-      <c r="B32" s="26">
+      <c r="B32" s="31">
         <f>B26+7</f>
         <v>45924</v>
       </c>
@@ -1236,28 +1245,28 @@
     </row>
     <row r="33" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
-      <c r="B33" s="27"/>
+      <c r="B33" s="32"/>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
       <c r="E33" s="8"/>
     </row>
     <row r="34" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
-      <c r="B34" s="27"/>
+      <c r="B34" s="32"/>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
       <c r="E34" s="8"/>
     </row>
     <row r="35" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
-      <c r="B35" s="27"/>
+      <c r="B35" s="32"/>
       <c r="C35" s="8"/>
       <c r="D35" s="9"/>
       <c r="E35" s="8"/>
     </row>
     <row r="36" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
-      <c r="B36" s="28"/>
+      <c r="B36" s="33"/>
       <c r="C36" s="8"/>
       <c r="D36" s="9"/>
       <c r="E36" s="8"/>
@@ -1266,14 +1275,14 @@
       <c r="A37" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="29"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="31"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="36"/>
     </row>
     <row r="38" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="26">
+      <c r="B38" s="31">
         <f>B32+7</f>
         <v>45931</v>
       </c>
@@ -1283,28 +1292,28 @@
     </row>
     <row r="39" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="27"/>
+      <c r="B39" s="32"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="27"/>
+      <c r="B40" s="32"/>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="27"/>
+      <c r="B41" s="32"/>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
-      <c r="B42" s="28"/>
+      <c r="B42" s="33"/>
       <c r="C42" s="10"/>
       <c r="D42" s="11"/>
       <c r="E42" s="10"/>
@@ -1313,14 +1322,14 @@
       <c r="A43" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="29"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30"/>
-      <c r="E43" s="31"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="36"/>
     </row>
     <row r="44" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
-      <c r="B44" s="26">
+      <c r="B44" s="31">
         <f>B38+7</f>
         <v>45938</v>
       </c>
@@ -1330,28 +1339,28 @@
     </row>
     <row r="45" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
-      <c r="B45" s="27"/>
+      <c r="B45" s="32"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
       <c r="E45" s="8"/>
     </row>
     <row r="46" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
-      <c r="B46" s="27"/>
+      <c r="B46" s="32"/>
       <c r="C46" s="8"/>
       <c r="D46" s="9"/>
       <c r="E46" s="8"/>
     </row>
     <row r="47" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
-      <c r="B47" s="27"/>
+      <c r="B47" s="32"/>
       <c r="C47" s="8"/>
       <c r="D47" s="9"/>
       <c r="E47" s="8"/>
     </row>
     <row r="48" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="10"/>
-      <c r="B48" s="28"/>
+      <c r="B48" s="33"/>
       <c r="C48" s="10"/>
       <c r="D48" s="11"/>
       <c r="E48" s="10"/>
@@ -1360,14 +1369,14 @@
       <c r="A49" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="29"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="30"/>
-      <c r="E49" s="31"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="36"/>
     </row>
     <row r="50" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
-      <c r="B50" s="26">
+      <c r="B50" s="31">
         <f>B44+7</f>
         <v>45945</v>
       </c>
@@ -1377,28 +1386,28 @@
     </row>
     <row r="51" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
-      <c r="B51" s="27"/>
+      <c r="B51" s="32"/>
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
       <c r="E51" s="8"/>
     </row>
     <row r="52" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
-      <c r="B52" s="27"/>
+      <c r="B52" s="32"/>
       <c r="C52" s="8"/>
       <c r="D52" s="9"/>
       <c r="E52" s="8"/>
     </row>
     <row r="53" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
-      <c r="B53" s="27"/>
+      <c r="B53" s="32"/>
       <c r="C53" s="8"/>
       <c r="D53" s="9"/>
       <c r="E53" s="8"/>
     </row>
     <row r="54" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="10"/>
-      <c r="B54" s="28"/>
+      <c r="B54" s="33"/>
       <c r="C54" s="10"/>
       <c r="D54" s="11"/>
       <c r="E54" s="10"/>
@@ -1407,14 +1416,14 @@
       <c r="A55" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="29"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="30"/>
-      <c r="E55" s="31"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="35"/>
+      <c r="E55" s="36"/>
     </row>
     <row r="56" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
-      <c r="B56" s="26">
+      <c r="B56" s="31">
         <f>B50+7</f>
         <v>45952</v>
       </c>
@@ -1424,28 +1433,28 @@
     </row>
     <row r="57" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
-      <c r="B57" s="27"/>
+      <c r="B57" s="32"/>
       <c r="C57" s="8"/>
       <c r="D57" s="9"/>
       <c r="E57" s="8"/>
     </row>
     <row r="58" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
-      <c r="B58" s="27"/>
+      <c r="B58" s="32"/>
       <c r="C58" s="8"/>
       <c r="D58" s="9"/>
       <c r="E58" s="8"/>
     </row>
     <row r="59" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
-      <c r="B59" s="27"/>
+      <c r="B59" s="32"/>
       <c r="C59" s="8"/>
       <c r="D59" s="9"/>
       <c r="E59" s="8"/>
     </row>
     <row r="60" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="10"/>
-      <c r="B60" s="28"/>
+      <c r="B60" s="33"/>
       <c r="C60" s="10"/>
       <c r="D60" s="11"/>
       <c r="E60" s="10"/>
@@ -1454,14 +1463,14 @@
       <c r="A61" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B61" s="29"/>
-      <c r="C61" s="30"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="31"/>
+      <c r="B61" s="34"/>
+      <c r="C61" s="35"/>
+      <c r="D61" s="35"/>
+      <c r="E61" s="36"/>
     </row>
     <row r="62" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
-      <c r="B62" s="26">
+      <c r="B62" s="31">
         <f>B56+7</f>
         <v>45959</v>
       </c>
@@ -1471,28 +1480,28 @@
     </row>
     <row r="63" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
-      <c r="B63" s="27"/>
+      <c r="B63" s="32"/>
       <c r="C63" s="8"/>
       <c r="D63" s="9"/>
       <c r="E63" s="8"/>
     </row>
     <row r="64" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
-      <c r="B64" s="27"/>
+      <c r="B64" s="32"/>
       <c r="C64" s="8"/>
       <c r="D64" s="9"/>
       <c r="E64" s="8"/>
     </row>
     <row r="65" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
-      <c r="B65" s="27"/>
+      <c r="B65" s="32"/>
       <c r="C65" s="8"/>
       <c r="D65" s="9"/>
       <c r="E65" s="8"/>
     </row>
     <row r="66" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8"/>
-      <c r="B66" s="28"/>
+      <c r="B66" s="33"/>
       <c r="C66" s="8"/>
       <c r="D66" s="9"/>
       <c r="E66" s="8"/>
@@ -1501,19 +1510,19 @@
       <c r="A67" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B67" s="29"/>
-      <c r="C67" s="30"/>
-      <c r="D67" s="30"/>
-      <c r="E67" s="31"/>
+      <c r="B67" s="34"/>
+      <c r="C67" s="35"/>
+      <c r="D67" s="35"/>
+      <c r="E67" s="36"/>
     </row>
     <row r="68" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="32" t="s">
+      <c r="A68" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B68" s="33"/>
+      <c r="B68" s="38"/>
       <c r="C68" s="15">
         <f>MROUND(SUM(C6:C67) /60,0.2)</f>
-        <v>6.6000000000000005</v>
+        <v>7.2</v>
       </c>
       <c r="D68" s="16"/>
       <c r="E68" s="17"/>
@@ -1528,6 +1537,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B50:B54"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B61:E61"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -1544,15 +1562,6 @@
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="B32:B36"/>
     <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B50:B54"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B61:E61"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C56:C60 C50:C54 C38:C42 C44:C48 C20:C24 B6 C12:C18 C26:C30 C32:C36 C62:C66 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
@@ -1582,15 +1591,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -1833,6 +1833,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1845,14 +1854,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1871,6 +1872,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
chore(jnr) : mise a jour du jnr
</commit_message>
<xml_diff>
--- a/doc/m-planification-jnltrav.xlsx
+++ b/doc/m-planification-jnltrav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Poo\P_oo-Shoot-me-up\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339B5419-18DC-4C15-A287-B9103762B327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D3BE94-B8DE-49B5-96F9-29044CA76DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t>Reprise des user story pour satisfaire au commantaire</t>
+  </si>
+  <si>
+    <t>Maquette</t>
+  </si>
+  <si>
+    <t>Nouvelle maquette pour le comportement des déplacement du joueur</t>
   </si>
 </sst>
 </file>
@@ -508,18 +514,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -549,6 +543,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -871,7 +877,7 @@
       <pane xSplit="3" ySplit="5" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -890,10 +896,10 @@
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="27"/>
+      <c r="C1" s="35"/>
       <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
@@ -905,10 +911,10 @@
       <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="22" t="s">
         <v>4</v>
       </c>
@@ -920,10 +926,10 @@
       <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="27"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="22" t="s">
         <v>7</v>
       </c>
@@ -935,12 +941,12 @@
       <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="38"/>
     </row>
     <row r="5" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -963,7 +969,7 @@
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="27">
         <v>45896</v>
       </c>
       <c r="C6" s="5">
@@ -978,7 +984,7 @@
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="32"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="8">
         <v>45</v>
       </c>
@@ -991,7 +997,7 @@
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="32"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="8">
         <v>45</v>
       </c>
@@ -1004,14 +1010,14 @@
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="32"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="33"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="10"/>
@@ -1020,16 +1026,16 @@
       <c r="A11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="36"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="32"/>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="27">
         <f>B6+7</f>
         <v>45903</v>
       </c>
@@ -1045,7 +1051,7 @@
       <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="32"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="8">
         <v>5</v>
       </c>
@@ -1058,7 +1064,7 @@
       <c r="A14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="32"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="8">
         <v>100</v>
       </c>
@@ -1074,7 +1080,7 @@
       <c r="A15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="32"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="8">
         <v>40</v>
       </c>
@@ -1089,7 +1095,7 @@
       <c r="A16" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="32"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="10">
         <v>5</v>
       </c>
@@ -1102,7 +1108,7 @@
       <c r="A17" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="32"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="10">
         <v>5</v>
       </c>
@@ -1113,7 +1119,7 @@
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
-      <c r="B18" s="33"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
       <c r="E18" s="10"/>
@@ -1122,16 +1128,16 @@
       <c r="A19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="36"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="32"/>
     </row>
     <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="31">
+      <c r="B20" s="27">
         <f>B12+7</f>
         <v>45910</v>
       </c>
@@ -1147,7 +1153,7 @@
       <c r="A21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="32"/>
+      <c r="B21" s="28"/>
       <c r="C21" s="8">
         <v>30</v>
       </c>
@@ -1157,22 +1163,28 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="8"/>
+      <c r="A22" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="28"/>
+      <c r="C22" s="8">
+        <v>15</v>
+      </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="8"/>
+      <c r="E22" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
-      <c r="B23" s="32"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="8"/>
       <c r="D23" s="9"/>
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
-      <c r="B24" s="33"/>
+      <c r="B24" s="29"/>
       <c r="C24" s="10"/>
       <c r="D24" s="11"/>
       <c r="E24" s="10"/>
@@ -1181,14 +1193,14 @@
       <c r="A25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="36"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="32"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="31">
+      <c r="B26" s="27">
         <f>B20+7</f>
         <v>45917</v>
       </c>
@@ -1198,28 +1210,28 @@
     </row>
     <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
-      <c r="B27" s="32"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="8"/>
       <c r="D27" s="9"/>
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
-      <c r="B28" s="32"/>
+      <c r="B28" s="28"/>
       <c r="C28" s="8"/>
       <c r="D28" s="9"/>
       <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
-      <c r="B29" s="32"/>
+      <c r="B29" s="28"/>
       <c r="C29" s="8"/>
       <c r="D29" s="9"/>
       <c r="E29" s="8"/>
     </row>
     <row r="30" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
-      <c r="B30" s="33"/>
+      <c r="B30" s="29"/>
       <c r="C30" s="10"/>
       <c r="D30" s="11"/>
       <c r="E30" s="10"/>
@@ -1228,14 +1240,14 @@
       <c r="A31" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="36"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="32"/>
     </row>
     <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
-      <c r="B32" s="31">
+      <c r="B32" s="27">
         <f>B26+7</f>
         <v>45924</v>
       </c>
@@ -1245,28 +1257,28 @@
     </row>
     <row r="33" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
-      <c r="B33" s="32"/>
+      <c r="B33" s="28"/>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
       <c r="E33" s="8"/>
     </row>
     <row r="34" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
-      <c r="B34" s="32"/>
+      <c r="B34" s="28"/>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
       <c r="E34" s="8"/>
     </row>
     <row r="35" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
-      <c r="B35" s="32"/>
+      <c r="B35" s="28"/>
       <c r="C35" s="8"/>
       <c r="D35" s="9"/>
       <c r="E35" s="8"/>
     </row>
     <row r="36" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
-      <c r="B36" s="33"/>
+      <c r="B36" s="29"/>
       <c r="C36" s="8"/>
       <c r="D36" s="9"/>
       <c r="E36" s="8"/>
@@ -1275,14 +1287,14 @@
       <c r="A37" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="36"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="32"/>
     </row>
     <row r="38" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="31">
+      <c r="B38" s="27">
         <f>B32+7</f>
         <v>45931</v>
       </c>
@@ -1292,28 +1304,28 @@
     </row>
     <row r="39" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="32"/>
+      <c r="B39" s="28"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="32"/>
+      <c r="B40" s="28"/>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="32"/>
+      <c r="B41" s="28"/>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
-      <c r="B42" s="33"/>
+      <c r="B42" s="29"/>
       <c r="C42" s="10"/>
       <c r="D42" s="11"/>
       <c r="E42" s="10"/>
@@ -1322,14 +1334,14 @@
       <c r="A43" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="34"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="36"/>
+      <c r="B43" s="30"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="32"/>
     </row>
     <row r="44" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
-      <c r="B44" s="31">
+      <c r="B44" s="27">
         <f>B38+7</f>
         <v>45938</v>
       </c>
@@ -1339,28 +1351,28 @@
     </row>
     <row r="45" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
-      <c r="B45" s="32"/>
+      <c r="B45" s="28"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
       <c r="E45" s="8"/>
     </row>
     <row r="46" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
-      <c r="B46" s="32"/>
+      <c r="B46" s="28"/>
       <c r="C46" s="8"/>
       <c r="D46" s="9"/>
       <c r="E46" s="8"/>
     </row>
     <row r="47" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
-      <c r="B47" s="32"/>
+      <c r="B47" s="28"/>
       <c r="C47" s="8"/>
       <c r="D47" s="9"/>
       <c r="E47" s="8"/>
     </row>
     <row r="48" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="10"/>
-      <c r="B48" s="33"/>
+      <c r="B48" s="29"/>
       <c r="C48" s="10"/>
       <c r="D48" s="11"/>
       <c r="E48" s="10"/>
@@ -1369,14 +1381,14 @@
       <c r="A49" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="34"/>
-      <c r="C49" s="35"/>
-      <c r="D49" s="35"/>
-      <c r="E49" s="36"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="32"/>
     </row>
     <row r="50" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
-      <c r="B50" s="31">
+      <c r="B50" s="27">
         <f>B44+7</f>
         <v>45945</v>
       </c>
@@ -1386,28 +1398,28 @@
     </row>
     <row r="51" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
-      <c r="B51" s="32"/>
+      <c r="B51" s="28"/>
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
       <c r="E51" s="8"/>
     </row>
     <row r="52" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
-      <c r="B52" s="32"/>
+      <c r="B52" s="28"/>
       <c r="C52" s="8"/>
       <c r="D52" s="9"/>
       <c r="E52" s="8"/>
     </row>
     <row r="53" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
-      <c r="B53" s="32"/>
+      <c r="B53" s="28"/>
       <c r="C53" s="8"/>
       <c r="D53" s="9"/>
       <c r="E53" s="8"/>
     </row>
     <row r="54" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="10"/>
-      <c r="B54" s="33"/>
+      <c r="B54" s="29"/>
       <c r="C54" s="10"/>
       <c r="D54" s="11"/>
       <c r="E54" s="10"/>
@@ -1416,14 +1428,14 @@
       <c r="A55" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="34"/>
-      <c r="C55" s="35"/>
-      <c r="D55" s="35"/>
-      <c r="E55" s="36"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="32"/>
     </row>
     <row r="56" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
-      <c r="B56" s="31">
+      <c r="B56" s="27">
         <f>B50+7</f>
         <v>45952</v>
       </c>
@@ -1433,28 +1445,28 @@
     </row>
     <row r="57" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
-      <c r="B57" s="32"/>
+      <c r="B57" s="28"/>
       <c r="C57" s="8"/>
       <c r="D57" s="9"/>
       <c r="E57" s="8"/>
     </row>
     <row r="58" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
-      <c r="B58" s="32"/>
+      <c r="B58" s="28"/>
       <c r="C58" s="8"/>
       <c r="D58" s="9"/>
       <c r="E58" s="8"/>
     </row>
     <row r="59" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
-      <c r="B59" s="32"/>
+      <c r="B59" s="28"/>
       <c r="C59" s="8"/>
       <c r="D59" s="9"/>
       <c r="E59" s="8"/>
     </row>
     <row r="60" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="10"/>
-      <c r="B60" s="33"/>
+      <c r="B60" s="29"/>
       <c r="C60" s="10"/>
       <c r="D60" s="11"/>
       <c r="E60" s="10"/>
@@ -1463,14 +1475,14 @@
       <c r="A61" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B61" s="34"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="35"/>
-      <c r="E61" s="36"/>
+      <c r="B61" s="30"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="32"/>
     </row>
     <row r="62" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
-      <c r="B62" s="31">
+      <c r="B62" s="27">
         <f>B56+7</f>
         <v>45959</v>
       </c>
@@ -1480,28 +1492,28 @@
     </row>
     <row r="63" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
-      <c r="B63" s="32"/>
+      <c r="B63" s="28"/>
       <c r="C63" s="8"/>
       <c r="D63" s="9"/>
       <c r="E63" s="8"/>
     </row>
     <row r="64" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
-      <c r="B64" s="32"/>
+      <c r="B64" s="28"/>
       <c r="C64" s="8"/>
       <c r="D64" s="9"/>
       <c r="E64" s="8"/>
     </row>
     <row r="65" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
-      <c r="B65" s="32"/>
+      <c r="B65" s="28"/>
       <c r="C65" s="8"/>
       <c r="D65" s="9"/>
       <c r="E65" s="8"/>
     </row>
     <row r="66" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8"/>
-      <c r="B66" s="33"/>
+      <c r="B66" s="29"/>
       <c r="C66" s="8"/>
       <c r="D66" s="9"/>
       <c r="E66" s="8"/>
@@ -1510,19 +1522,19 @@
       <c r="A67" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B67" s="34"/>
-      <c r="C67" s="35"/>
-      <c r="D67" s="35"/>
-      <c r="E67" s="36"/>
+      <c r="B67" s="30"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="32"/>
     </row>
     <row r="68" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="37" t="s">
+      <c r="A68" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B68" s="38"/>
+      <c r="B68" s="34"/>
       <c r="C68" s="15">
         <f>MROUND(SUM(C6:C67) /60,0.2)</f>
-        <v>7.2</v>
+        <v>7.4</v>
       </c>
       <c r="D68" s="16"/>
       <c r="E68" s="17"/>
@@ -1537,15 +1549,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B50:B54"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B61:E61"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -1562,6 +1565,15 @@
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="B32:B36"/>
     <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B50:B54"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B61:E61"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C56:C60 C50:C54 C38:C42 C44:C48 C20:C24 B6 C12:C18 C26:C30 C32:C36 C62:C66 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
@@ -1591,6 +1603,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -1833,15 +1854,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1854,6 +1866,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1872,14 +1892,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
chore(jnr) : modif du jnr
</commit_message>
<xml_diff>
--- a/doc/m-planification-jnltrav.xlsx
+++ b/doc/m-planification-jnltrav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Poo\P_oo-Shoot-me-up\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D3BE94-B8DE-49B5-96F9-29044CA76DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1D4E03-3D67-4FA9-8AF1-D1F8FADA4ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -188,6 +188,18 @@
   </si>
   <si>
     <t>Nouvelle maquette pour le comportement des déplacement du joueur</t>
+  </si>
+  <si>
+    <t>Explication</t>
+  </si>
+  <si>
+    <t>Comment débuter le projet en FORM</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Affichage du fond et du joueur</t>
   </si>
 </sst>
 </file>
@@ -877,7 +889,7 @@
       <pane xSplit="3" ySplit="5" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomRight" activeCell="B25" sqref="B25:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1168,7 +1180,7 @@
       </c>
       <c r="B22" s="28"/>
       <c r="C22" s="8">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="8" t="s">
@@ -1176,18 +1188,30 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
+      <c r="A23" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="B23" s="28"/>
-      <c r="C23" s="8"/>
+      <c r="C23" s="8">
+        <v>30</v>
+      </c>
       <c r="D23" s="9"/>
-      <c r="E23" s="8"/>
+      <c r="E23" s="8" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
+      <c r="A24" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="B24" s="29"/>
-      <c r="C24" s="10"/>
+      <c r="C24" s="10">
+        <v>60</v>
+      </c>
       <c r="D24" s="11"/>
-      <c r="E24" s="10"/>
+      <c r="E24" s="10" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
@@ -1534,7 +1558,7 @@
       <c r="B68" s="34"/>
       <c r="C68" s="15">
         <f>MROUND(SUM(C6:C67) /60,0.2)</f>
-        <v>7.4</v>
+        <v>9</v>
       </c>
       <c r="D68" s="16"/>
       <c r="E68" s="17"/>

</xml_diff>

<commit_message>
Fix(joueur) : Placement du joueur
[20min] [Done]
</commit_message>
<xml_diff>
--- a/doc/m-planification-jnltrav.xlsx
+++ b/doc/m-planification-jnltrav.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Poo\P_oo-Shoot-me-up\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1D4E03-3D67-4FA9-8AF1-D1F8FADA4ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7C70EE-C426-4AD9-B712-73D3A57EB8B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -200,6 +200,15 @@
   </si>
   <si>
     <t>Affichage du fond et du joueur</t>
+  </si>
+  <si>
+    <t>Déplacment</t>
+  </si>
+  <si>
+    <t>Déplacement du joueur avec tous les problemes qui on suivit</t>
+  </si>
+  <si>
+    <t>Explication des déplacement par Tony + celle du prof</t>
   </si>
 </sst>
 </file>
@@ -526,6 +535,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -555,18 +576,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -886,10 +895,10 @@
   <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="E10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B25" sqref="B25:E25"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -908,10 +917,10 @@
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="35"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
@@ -923,10 +932,10 @@
       <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="35"/>
+      <c r="C2" s="27"/>
       <c r="D2" s="22" t="s">
         <v>4</v>
       </c>
@@ -938,10 +947,10 @@
       <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="35"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="22" t="s">
         <v>7</v>
       </c>
@@ -953,12 +962,12 @@
       <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="38"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -981,7 +990,7 @@
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="31">
         <v>45896</v>
       </c>
       <c r="C6" s="5">
@@ -996,7 +1005,7 @@
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="28"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="8">
         <v>45</v>
       </c>
@@ -1009,7 +1018,7 @@
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="28"/>
+      <c r="B8" s="32"/>
       <c r="C8" s="8">
         <v>45</v>
       </c>
@@ -1022,14 +1031,14 @@
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="28"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="29"/>
+      <c r="B10" s="33"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="10"/>
@@ -1038,16 +1047,16 @@
       <c r="A11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="27">
+      <c r="B12" s="31">
         <f>B6+7</f>
         <v>45903</v>
       </c>
@@ -1063,7 +1072,7 @@
       <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="28"/>
+      <c r="B13" s="32"/>
       <c r="C13" s="8">
         <v>5</v>
       </c>
@@ -1076,7 +1085,7 @@
       <c r="A14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="28"/>
+      <c r="B14" s="32"/>
       <c r="C14" s="8">
         <v>100</v>
       </c>
@@ -1092,7 +1101,7 @@
       <c r="A15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="28"/>
+      <c r="B15" s="32"/>
       <c r="C15" s="8">
         <v>40</v>
       </c>
@@ -1107,7 +1116,7 @@
       <c r="A16" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="28"/>
+      <c r="B16" s="32"/>
       <c r="C16" s="10">
         <v>5</v>
       </c>
@@ -1120,7 +1129,7 @@
       <c r="A17" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="28"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="10">
         <v>5</v>
       </c>
@@ -1131,7 +1140,7 @@
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
-      <c r="B18" s="29"/>
+      <c r="B18" s="33"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
       <c r="E18" s="10"/>
@@ -1140,16 +1149,16 @@
       <c r="A19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="32"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="36"/>
     </row>
     <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="27">
+      <c r="B20" s="31">
         <f>B12+7</f>
         <v>45910</v>
       </c>
@@ -1165,7 +1174,7 @@
       <c r="A21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="28"/>
+      <c r="B21" s="32"/>
       <c r="C21" s="8">
         <v>30</v>
       </c>
@@ -1178,7 +1187,7 @@
       <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="28"/>
+      <c r="B22" s="32"/>
       <c r="C22" s="8">
         <v>20</v>
       </c>
@@ -1191,7 +1200,7 @@
       <c r="A23" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="28"/>
+      <c r="B23" s="32"/>
       <c r="C23" s="8">
         <v>30</v>
       </c>
@@ -1204,7 +1213,7 @@
       <c r="A24" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="29"/>
+      <c r="B24" s="33"/>
       <c r="C24" s="10">
         <v>60</v>
       </c>
@@ -1217,45 +1226,57 @@
       <c r="A25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="32"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="36"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="27">
+      <c r="A26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="31">
         <f>B20+7</f>
         <v>45917</v>
       </c>
-      <c r="C26" s="5"/>
+      <c r="C26" s="5">
+        <v>50</v>
+      </c>
       <c r="D26" s="6"/>
-      <c r="E26" s="5"/>
+      <c r="E26" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="8"/>
+      <c r="A27" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="32"/>
+      <c r="C27" s="8">
+        <v>20</v>
+      </c>
       <c r="D27" s="9"/>
-      <c r="E27" s="8"/>
+      <c r="E27" s="8" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
-      <c r="B28" s="28"/>
+      <c r="B28" s="32"/>
       <c r="C28" s="8"/>
       <c r="D28" s="9"/>
       <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
-      <c r="B29" s="28"/>
+      <c r="B29" s="32"/>
       <c r="C29" s="8"/>
       <c r="D29" s="9"/>
       <c r="E29" s="8"/>
     </row>
     <row r="30" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
-      <c r="B30" s="29"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="10"/>
       <c r="D30" s="11"/>
       <c r="E30" s="10"/>
@@ -1264,14 +1285,14 @@
       <c r="A31" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="32"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="36"/>
     </row>
     <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
-      <c r="B32" s="27">
+      <c r="B32" s="31">
         <f>B26+7</f>
         <v>45924</v>
       </c>
@@ -1281,28 +1302,28 @@
     </row>
     <row r="33" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
-      <c r="B33" s="28"/>
+      <c r="B33" s="32"/>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
       <c r="E33" s="8"/>
     </row>
     <row r="34" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
-      <c r="B34" s="28"/>
+      <c r="B34" s="32"/>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
       <c r="E34" s="8"/>
     </row>
     <row r="35" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
-      <c r="B35" s="28"/>
+      <c r="B35" s="32"/>
       <c r="C35" s="8"/>
       <c r="D35" s="9"/>
       <c r="E35" s="8"/>
     </row>
     <row r="36" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
-      <c r="B36" s="29"/>
+      <c r="B36" s="33"/>
       <c r="C36" s="8"/>
       <c r="D36" s="9"/>
       <c r="E36" s="8"/>
@@ -1311,14 +1332,14 @@
       <c r="A37" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="32"/>
+      <c r="B37" s="34"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="36"/>
     </row>
     <row r="38" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
-      <c r="B38" s="27">
+      <c r="B38" s="31">
         <f>B32+7</f>
         <v>45931</v>
       </c>
@@ -1328,28 +1349,28 @@
     </row>
     <row r="39" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
-      <c r="B39" s="28"/>
+      <c r="B39" s="32"/>
       <c r="C39" s="8"/>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
-      <c r="B40" s="28"/>
+      <c r="B40" s="32"/>
       <c r="C40" s="8"/>
       <c r="D40" s="9"/>
       <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
-      <c r="B41" s="28"/>
+      <c r="B41" s="32"/>
       <c r="C41" s="8"/>
       <c r="D41" s="9"/>
       <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10"/>
-      <c r="B42" s="29"/>
+      <c r="B42" s="33"/>
       <c r="C42" s="10"/>
       <c r="D42" s="11"/>
       <c r="E42" s="10"/>
@@ -1358,14 +1379,14 @@
       <c r="A43" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="30"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="32"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="36"/>
     </row>
     <row r="44" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
-      <c r="B44" s="27">
+      <c r="B44" s="31">
         <f>B38+7</f>
         <v>45938</v>
       </c>
@@ -1375,28 +1396,28 @@
     </row>
     <row r="45" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
-      <c r="B45" s="28"/>
+      <c r="B45" s="32"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
       <c r="E45" s="8"/>
     </row>
     <row r="46" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
-      <c r="B46" s="28"/>
+      <c r="B46" s="32"/>
       <c r="C46" s="8"/>
       <c r="D46" s="9"/>
       <c r="E46" s="8"/>
     </row>
     <row r="47" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
-      <c r="B47" s="28"/>
+      <c r="B47" s="32"/>
       <c r="C47" s="8"/>
       <c r="D47" s="9"/>
       <c r="E47" s="8"/>
     </row>
     <row r="48" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="10"/>
-      <c r="B48" s="29"/>
+      <c r="B48" s="33"/>
       <c r="C48" s="10"/>
       <c r="D48" s="11"/>
       <c r="E48" s="10"/>
@@ -1405,14 +1426,14 @@
       <c r="A49" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="30"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="32"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="35"/>
+      <c r="E49" s="36"/>
     </row>
     <row r="50" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
-      <c r="B50" s="27">
+      <c r="B50" s="31">
         <f>B44+7</f>
         <v>45945</v>
       </c>
@@ -1422,28 +1443,28 @@
     </row>
     <row r="51" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
-      <c r="B51" s="28"/>
+      <c r="B51" s="32"/>
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
       <c r="E51" s="8"/>
     </row>
     <row r="52" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
-      <c r="B52" s="28"/>
+      <c r="B52" s="32"/>
       <c r="C52" s="8"/>
       <c r="D52" s="9"/>
       <c r="E52" s="8"/>
     </row>
     <row r="53" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
-      <c r="B53" s="28"/>
+      <c r="B53" s="32"/>
       <c r="C53" s="8"/>
       <c r="D53" s="9"/>
       <c r="E53" s="8"/>
     </row>
     <row r="54" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="10"/>
-      <c r="B54" s="29"/>
+      <c r="B54" s="33"/>
       <c r="C54" s="10"/>
       <c r="D54" s="11"/>
       <c r="E54" s="10"/>
@@ -1452,14 +1473,14 @@
       <c r="A55" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="32"/>
+      <c r="B55" s="34"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="35"/>
+      <c r="E55" s="36"/>
     </row>
     <row r="56" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
-      <c r="B56" s="27">
+      <c r="B56" s="31">
         <f>B50+7</f>
         <v>45952</v>
       </c>
@@ -1469,28 +1490,28 @@
     </row>
     <row r="57" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
-      <c r="B57" s="28"/>
+      <c r="B57" s="32"/>
       <c r="C57" s="8"/>
       <c r="D57" s="9"/>
       <c r="E57" s="8"/>
     </row>
     <row r="58" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
-      <c r="B58" s="28"/>
+      <c r="B58" s="32"/>
       <c r="C58" s="8"/>
       <c r="D58" s="9"/>
       <c r="E58" s="8"/>
     </row>
     <row r="59" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
-      <c r="B59" s="28"/>
+      <c r="B59" s="32"/>
       <c r="C59" s="8"/>
       <c r="D59" s="9"/>
       <c r="E59" s="8"/>
     </row>
     <row r="60" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="10"/>
-      <c r="B60" s="29"/>
+      <c r="B60" s="33"/>
       <c r="C60" s="10"/>
       <c r="D60" s="11"/>
       <c r="E60" s="10"/>
@@ -1499,14 +1520,14 @@
       <c r="A61" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B61" s="30"/>
-      <c r="C61" s="31"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="32"/>
+      <c r="B61" s="34"/>
+      <c r="C61" s="35"/>
+      <c r="D61" s="35"/>
+      <c r="E61" s="36"/>
     </row>
     <row r="62" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
-      <c r="B62" s="27">
+      <c r="B62" s="31">
         <f>B56+7</f>
         <v>45959</v>
       </c>
@@ -1516,28 +1537,28 @@
     </row>
     <row r="63" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
-      <c r="B63" s="28"/>
+      <c r="B63" s="32"/>
       <c r="C63" s="8"/>
       <c r="D63" s="9"/>
       <c r="E63" s="8"/>
     </row>
     <row r="64" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
-      <c r="B64" s="28"/>
+      <c r="B64" s="32"/>
       <c r="C64" s="8"/>
       <c r="D64" s="9"/>
       <c r="E64" s="8"/>
     </row>
     <row r="65" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
-      <c r="B65" s="28"/>
+      <c r="B65" s="32"/>
       <c r="C65" s="8"/>
       <c r="D65" s="9"/>
       <c r="E65" s="8"/>
     </row>
     <row r="66" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="8"/>
-      <c r="B66" s="29"/>
+      <c r="B66" s="33"/>
       <c r="C66" s="8"/>
       <c r="D66" s="9"/>
       <c r="E66" s="8"/>
@@ -1546,19 +1567,19 @@
       <c r="A67" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B67" s="30"/>
-      <c r="C67" s="31"/>
-      <c r="D67" s="31"/>
-      <c r="E67" s="32"/>
+      <c r="B67" s="34"/>
+      <c r="C67" s="35"/>
+      <c r="D67" s="35"/>
+      <c r="E67" s="36"/>
     </row>
     <row r="68" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="33" t="s">
+      <c r="A68" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B68" s="34"/>
+      <c r="B68" s="38"/>
       <c r="C68" s="15">
         <f>MROUND(SUM(C6:C67) /60,0.2)</f>
-        <v>9</v>
+        <v>10.200000000000001</v>
       </c>
       <c r="D68" s="16"/>
       <c r="E68" s="17"/>
@@ -1573,6 +1594,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="B50:B54"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B61:E61"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -1589,15 +1619,6 @@
     <mergeCell ref="B31:E31"/>
     <mergeCell ref="B32:B36"/>
     <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B50:B54"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B61:E61"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C56:C60 C50:C54 C38:C42 C44:C48 C20:C24 B6 C12:C18 C26:C30 C32:C36 C62:C66 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
@@ -1627,15 +1648,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -1878,6 +1890,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1890,14 +1911,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1916,6 +1929,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fix(PV) : centrage des pv
[10min] [Done]
</commit_message>
<xml_diff>
--- a/doc/m-planification-jnltrav.xlsx
+++ b/doc/m-planification-jnltrav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Poo\P_oo-Shoot-me-up\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7C70EE-C426-4AD9-B712-73D3A57EB8B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05C9103-758E-48C7-B804-F0933A16A5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -209,6 +209,18 @@
   </si>
   <si>
     <t>Explication des déplacement par Tony + celle du prof</t>
+  </si>
+  <si>
+    <t>Placement</t>
+  </si>
+  <si>
+    <t>Placment du joueur au debut</t>
+  </si>
+  <si>
+    <t>point de vie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affichage de la vie </t>
   </si>
 </sst>
 </file>
@@ -895,10 +907,10 @@
   <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="E22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1261,18 +1273,30 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+      <c r="A28" s="7" t="s">
+        <v>53</v>
+      </c>
       <c r="B28" s="32"/>
-      <c r="C28" s="8"/>
+      <c r="C28" s="8">
+        <v>20</v>
+      </c>
       <c r="D28" s="9"/>
-      <c r="E28" s="8"/>
+      <c r="E28" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
+      <c r="A29" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="B29" s="32"/>
-      <c r="C29" s="8"/>
+      <c r="C29" s="8">
+        <v>10</v>
+      </c>
       <c r="D29" s="9"/>
-      <c r="E29" s="8"/>
+      <c r="E29" s="8" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
@@ -1579,7 +1603,7 @@
       <c r="B68" s="38"/>
       <c r="C68" s="15">
         <f>MROUND(SUM(C6:C67) /60,0.2)</f>
-        <v>10.200000000000001</v>
+        <v>10.600000000000001</v>
       </c>
       <c r="D68" s="16"/>
       <c r="E68" s="17"/>

</xml_diff>

<commit_message>
Chore(Commentaire) : comm inutile
</commit_message>
<xml_diff>
--- a/doc/m-planification-jnltrav.xlsx
+++ b/doc/m-planification-jnltrav.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Poo\P_oo-Shoot-me-up\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05C9103-758E-48C7-B804-F0933A16A5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998CBADE-3EB5-4A03-A87F-3617EB45946B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$68</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$72</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -221,6 +221,24 @@
   </si>
   <si>
     <t xml:space="preserve">Affichage de la vie </t>
+  </si>
+  <si>
+    <t>Ne peu plus entrer dans les mur</t>
+  </si>
+  <si>
+    <t>Cooldown des tire</t>
+  </si>
+  <si>
+    <t>Auto incremant des pv</t>
+  </si>
+  <si>
+    <t>Tire</t>
+  </si>
+  <si>
+    <t>Mur</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/fr-fr/dotnet/api/system.windows.markup.icomponentconnector.initializecomponent?view=windowsdesktop-9.0</t>
   </si>
 </sst>
 </file>
@@ -454,7 +472,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -547,6 +565,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -559,35 +607,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -904,13 +940,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="E22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -929,10 +965,10 @@
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="27"/>
+      <c r="C1" s="35"/>
       <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
@@ -944,10 +980,10 @@
       <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="22" t="s">
         <v>4</v>
       </c>
@@ -959,10 +995,10 @@
       <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="27"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="22" t="s">
         <v>7</v>
       </c>
@@ -974,12 +1010,12 @@
       <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="38"/>
     </row>
     <row r="5" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1002,7 +1038,7 @@
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="27">
         <v>45896</v>
       </c>
       <c r="C6" s="5">
@@ -1017,7 +1053,7 @@
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="32"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="8">
         <v>45</v>
       </c>
@@ -1030,7 +1066,7 @@
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="32"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="8">
         <v>45</v>
       </c>
@@ -1043,14 +1079,14 @@
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="32"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="33"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="10"/>
@@ -1059,16 +1095,16 @@
       <c r="A11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="36"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="32"/>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="27">
         <f>B6+7</f>
         <v>45903</v>
       </c>
@@ -1084,7 +1120,7 @@
       <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="32"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="8">
         <v>5</v>
       </c>
@@ -1097,7 +1133,7 @@
       <c r="A14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="32"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="8">
         <v>100</v>
       </c>
@@ -1113,7 +1149,7 @@
       <c r="A15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="32"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="8">
         <v>40</v>
       </c>
@@ -1128,7 +1164,7 @@
       <c r="A16" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="32"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="10">
         <v>5</v>
       </c>
@@ -1141,7 +1177,7 @@
       <c r="A17" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="32"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="10">
         <v>5</v>
       </c>
@@ -1152,7 +1188,7 @@
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
-      <c r="B18" s="33"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
       <c r="E18" s="10"/>
@@ -1161,24 +1197,23 @@
       <c r="A19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="36"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="32"/>
     </row>
     <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="31">
+      <c r="B20" s="27">
         <f>B12+7</f>
         <v>45910</v>
       </c>
       <c r="C20" s="5">
         <v>40</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1186,12 +1221,11 @@
       <c r="A21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="32"/>
+      <c r="B21" s="28"/>
       <c r="C21" s="8">
         <v>30</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="8" t="s">
+      <c r="D21" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1199,12 +1233,11 @@
       <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="32"/>
+      <c r="B22" s="28"/>
       <c r="C22" s="8">
         <v>20</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="8" t="s">
+      <c r="D22" s="8" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1212,12 +1245,11 @@
       <c r="A23" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="32"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="8">
         <v>30</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="8" t="s">
+      <c r="D23" s="8" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1225,12 +1257,11 @@
       <c r="A24" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="33"/>
+      <c r="B24" s="29"/>
       <c r="C24" s="10">
         <v>60</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="10" t="s">
+      <c r="D24" s="10" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1238,37 +1269,38 @@
       <c r="A25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="36"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="32"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="31">
+      <c r="B26" s="27">
         <f>B20+7</f>
         <v>45917</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="39">
         <v>50</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="5" t="s">
+      <c r="D26" s="40" t="s">
         <v>51</v>
+      </c>
+      <c r="E26" s="43" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="8">
+      <c r="B27" s="28"/>
+      <c r="C27" s="39">
         <v>20</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="8" t="s">
+      <c r="D27" s="41" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1276,379 +1308,414 @@
       <c r="A28" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="8">
+      <c r="B28" s="28"/>
+      <c r="C28" s="39">
         <v>20</v>
       </c>
-      <c r="D28" s="9"/>
-      <c r="E28" s="8" t="s">
+      <c r="D28" s="41" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="28"/>
+      <c r="C29" s="39">
+        <v>20</v>
+      </c>
+      <c r="D29" s="41" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="28"/>
+      <c r="C30" s="39">
+        <v>20</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="8">
+      <c r="B31" s="28"/>
+      <c r="C31" s="39">
         <v>10</v>
       </c>
-      <c r="D29" s="9"/>
-      <c r="E29" s="8" t="s">
+      <c r="D31" s="41" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="10"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="10"/>
-    </row>
-    <row r="31" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12" t="s">
+    <row r="32" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="29"/>
+      <c r="C32" s="39">
+        <v>10</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" s="10"/>
+    </row>
+    <row r="33" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="36"/>
-    </row>
-    <row r="32" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="31">
+      <c r="B33" s="30"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="32"/>
+    </row>
+    <row r="34" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="27">
         <f>B26+7</f>
         <v>45924</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="13"/>
-    </row>
-    <row r="33" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="8"/>
+      <c r="C34" s="39"/>
+      <c r="E34" s="13"/>
     </row>
     <row r="35" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="39"/>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
-      <c r="B36" s="33"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="39"/>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="12" t="s">
+    <row r="37" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="39"/>
+      <c r="E37" s="8"/>
+    </row>
+    <row r="38" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="39"/>
+      <c r="E38" s="8"/>
+    </row>
+    <row r="39" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="39"/>
+      <c r="E39" s="8"/>
+    </row>
+    <row r="40" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="8"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="39"/>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="36"/>
-    </row>
-    <row r="38" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="31">
-        <f>B32+7</f>
+      <c r="B41" s="30"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="32"/>
+    </row>
+    <row r="42" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="27">
+        <f>B34+7</f>
         <v>45931</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="8"/>
-    </row>
-    <row r="40" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="8"/>
-    </row>
-    <row r="41" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="8"/>
-    </row>
-    <row r="42" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="10"/>
-      <c r="B42" s="33"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="10"/>
-    </row>
-    <row r="43" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B43" s="34"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="36"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="8"/>
     </row>
     <row r="44" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="31">
-        <f>B38+7</f>
-        <v>45938</v>
-      </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="5"/>
+      <c r="A44" s="7"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="8"/>
     </row>
     <row r="45" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
-      <c r="B45" s="32"/>
+      <c r="B45" s="28"/>
       <c r="C45" s="8"/>
       <c r="D45" s="9"/>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="8"/>
-    </row>
-    <row r="47" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="32"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="8"/>
-    </row>
-    <row r="48" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="10"/>
-      <c r="B48" s="33"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="10"/>
-    </row>
-    <row r="49" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="12" t="s">
+    <row r="46" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="10"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="10"/>
+    </row>
+    <row r="47" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B49" s="34"/>
-      <c r="C49" s="35"/>
-      <c r="D49" s="35"/>
-      <c r="E49" s="36"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="32"/>
+    </row>
+    <row r="48" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="27">
+        <f>B42+7</f>
+        <v>45938</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="5"/>
+    </row>
+    <row r="49" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="7"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="8"/>
     </row>
     <row r="50" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="31">
-        <f>B44+7</f>
-        <v>45945</v>
-      </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="5"/>
+      <c r="A50" s="7"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="8"/>
     </row>
     <row r="51" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
-      <c r="B51" s="32"/>
+      <c r="B51" s="28"/>
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
       <c r="E51" s="8"/>
     </row>
-    <row r="52" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
-      <c r="B52" s="32"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="8"/>
-    </row>
-    <row r="53" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
-      <c r="B53" s="32"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="8"/>
-    </row>
-    <row r="54" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="10"/>
-      <c r="B54" s="33"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="10"/>
-    </row>
-    <row r="55" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="12" t="s">
+    <row r="52" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="10"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="10"/>
+    </row>
+    <row r="53" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="34"/>
-      <c r="C55" s="35"/>
-      <c r="D55" s="35"/>
-      <c r="E55" s="36"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="32"/>
+    </row>
+    <row r="54" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="27">
+        <f>B48+7</f>
+        <v>45945</v>
+      </c>
+      <c r="C54" s="5"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="5"/>
+    </row>
+    <row r="55" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="8"/>
     </row>
     <row r="56" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="31">
-        <f>B50+7</f>
-        <v>45952</v>
-      </c>
-      <c r="C56" s="5"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="5"/>
+      <c r="A56" s="7"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
-      <c r="B57" s="32"/>
+      <c r="B57" s="28"/>
       <c r="C57" s="8"/>
       <c r="D57" s="9"/>
       <c r="E57" s="8"/>
     </row>
-    <row r="58" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
-      <c r="B58" s="32"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="8"/>
-    </row>
-    <row r="59" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" s="32"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="8"/>
-    </row>
-    <row r="60" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="10"/>
-      <c r="B60" s="33"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="11"/>
-      <c r="E60" s="10"/>
-    </row>
-    <row r="61" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="12" t="s">
+    <row r="58" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="10"/>
+      <c r="B58" s="29"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="10"/>
+    </row>
+    <row r="59" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B61" s="34"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="35"/>
-      <c r="E61" s="36"/>
+      <c r="B59" s="30"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="32"/>
+    </row>
+    <row r="60" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="27">
+        <f>B54+7</f>
+        <v>45952</v>
+      </c>
+      <c r="C60" s="5"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="5"/>
+    </row>
+    <row r="61" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="7"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="8"/>
     </row>
     <row r="62" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
-      <c r="B62" s="31">
-        <f>B56+7</f>
-        <v>45959</v>
-      </c>
-      <c r="C62" s="13"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="13"/>
+      <c r="A62" s="7"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="8"/>
     </row>
     <row r="63" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="8"/>
-      <c r="B63" s="32"/>
+      <c r="A63" s="7"/>
+      <c r="B63" s="28"/>
       <c r="C63" s="8"/>
       <c r="D63" s="9"/>
       <c r="E63" s="8"/>
     </row>
-    <row r="64" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="8"/>
-      <c r="B64" s="32"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="8"/>
-    </row>
-    <row r="65" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="8"/>
-      <c r="B65" s="32"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="9"/>
-      <c r="E65" s="8"/>
-    </row>
-    <row r="66" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="8"/>
-      <c r="B66" s="33"/>
-      <c r="C66" s="8"/>
-      <c r="D66" s="9"/>
-      <c r="E66" s="8"/>
-    </row>
-    <row r="67" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="12" t="s">
+    <row r="64" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="10"/>
+      <c r="B64" s="29"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="10"/>
+    </row>
+    <row r="65" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B67" s="34"/>
-      <c r="C67" s="35"/>
-      <c r="D67" s="35"/>
-      <c r="E67" s="36"/>
-    </row>
-    <row r="68" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="37" t="s">
+      <c r="B65" s="30"/>
+      <c r="C65" s="31"/>
+      <c r="D65" s="31"/>
+      <c r="E65" s="32"/>
+    </row>
+    <row r="66" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
+      <c r="B66" s="27">
+        <f>B60+7</f>
+        <v>45959</v>
+      </c>
+      <c r="C66" s="13"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="13"/>
+    </row>
+    <row r="67" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="8"/>
+      <c r="B67" s="28"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="8"/>
+    </row>
+    <row r="68" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="8"/>
+      <c r="B68" s="28"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="8"/>
+    </row>
+    <row r="69" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="8"/>
+      <c r="B69" s="28"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="8"/>
+    </row>
+    <row r="70" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="8"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="8"/>
+    </row>
+    <row r="71" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B71" s="30"/>
+      <c r="C71" s="31"/>
+      <c r="D71" s="31"/>
+      <c r="E71" s="32"/>
+    </row>
+    <row r="72" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B68" s="38"/>
-      <c r="C68" s="15">
-        <f>MROUND(SUM(C6:C67) /60,0.2)</f>
-        <v>10.600000000000001</v>
-      </c>
-      <c r="D68" s="16"/>
-      <c r="E68" s="17"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="18" t="s">
+      <c r="B72" s="34"/>
+      <c r="C72" s="15">
+        <f>MROUND(SUM(C6:C71) /60,0.2)</f>
+        <v>11.600000000000001</v>
+      </c>
+      <c r="D72" s="16"/>
+      <c r="E72" s="17"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="18"/>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B38:B42"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="B50:B54"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B61:E61"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B62:B66"/>
-    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="B66:B70"/>
+    <mergeCell ref="B47:E47"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:B18"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B20:B24"/>
     <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B26:B32"/>
+    <mergeCell ref="B33:E33"/>
+    <mergeCell ref="B34:B40"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B42:B46"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="B48:B52"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="B54:B58"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="B60:B64"/>
+    <mergeCell ref="B65:E65"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C56:C60 C50:C54 C38:C42 C44:C48 C20:C24 B6 C12:C18 C26:C30 C32:C36 C62:C66 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C60:C64 C54:C58 C42:C46 C48:C52 C20:C24 B6 C12:C18 C66:C70 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B12:B18 B56:B60 B20:B24 B26:B30 B32:B36 B38:B42 B44:B48 B50:B54 B62:B66" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B12:B18 B60:B64 B20:B24 B26:B32 B34:B40 B42:B46 B48:B52 B54:B58 B66:B70" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
       <formula1>45261</formula1>
     </dataValidation>
   </dataValidations>
@@ -1656,10 +1723,11 @@
     <hyperlink ref="E14" r:id="rId1" display="| Backlog · kanban" xr:uid="{9B5D630F-F3CA-4BE9-BE1C-70C324722A61}"/>
     <hyperlink ref="E15" r:id="rId2" xr:uid="{B9AB9621-1570-41D7-A2C6-6FF27F13DC4B}"/>
     <hyperlink ref="E8" r:id="rId3" xr:uid="{8FEF73A3-AAC4-4357-865C-F89C66FF328B}"/>
+    <hyperlink ref="E26" r:id="rId4" xr:uid="{BA47B067-B875-4B68-9985-3024D1156F3F}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="37" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" scale="37" orientation="portrait" r:id="rId5"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Etml_font,Normal"&amp;22ETML&amp;R&amp;G</oddHeader>
     <oddFooter>&amp;L&amp;14&amp;D&amp;R&amp;14Journal</oddFooter>
@@ -1667,11 +1735,20 @@
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="17" max="16383" man="1"/>
   </rowBreaks>
-  <legacyDrawingHF r:id="rId5"/>
+  <legacyDrawingHF r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -1914,15 +1991,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1935,6 +2003,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1953,14 +2029,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
   <ds:schemaRefs>

</xml_diff>